<commit_message>
Spárovky a ukotvení botníku
</commit_message>
<xml_diff>
--- a/PCB NG/Plnění.xlsx
+++ b/PCB NG/Plnění.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\STL\PCB NG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052D57C3-80B0-4FF2-B2B9-441A9C5635A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0D44A8-43E4-4A48-B8C9-91B24FFC883B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0C12EAB3-5C5A-4529-92B3-802642319947}"/>
   </bookViews>
@@ -1724,7 +1724,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,11 +1781,11 @@
       </c>
       <c r="F2" s="11">
         <f>$B$10*E2</f>
-        <v>98.5</v>
+        <v>96.569400000000002</v>
       </c>
       <c r="G2" s="11">
         <f>$B$11*E2*$B$10</f>
-        <v>275.8</v>
+        <v>270.39431999999999</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1806,11 +1806,11 @@
       </c>
       <c r="F3" s="11">
         <f t="shared" ref="F3:F7" si="0">$B$10*E3</f>
-        <v>13.750000000000002</v>
+        <v>13.480500000000003</v>
       </c>
       <c r="G3" s="11">
         <f t="shared" ref="G3:G7" si="1">$B$11*E3*$B$10</f>
-        <v>38.5</v>
+        <v>37.745400000000004</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1831,11 +1831,11 @@
       </c>
       <c r="F4" s="11">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>4.6569000000000003</v>
       </c>
       <c r="G4" s="11">
         <f t="shared" si="1"/>
-        <v>13.299999999999997</v>
+        <v>13.039319999999998</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1856,11 +1856,11 @@
       </c>
       <c r="F5" s="11">
         <f t="shared" si="0"/>
-        <v>24.5</v>
+        <v>24.0198</v>
       </c>
       <c r="G5" s="11">
         <f t="shared" si="1"/>
-        <v>68.599999999999994</v>
+        <v>67.255439999999993</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1881,11 +1881,11 @@
       </c>
       <c r="F6" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3.9216000000000002</v>
       </c>
       <c r="G6" s="11">
         <f t="shared" si="1"/>
-        <v>11.2</v>
+        <v>10.98048</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1906,11 +1906,11 @@
       </c>
       <c r="F7" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.9412000000000003</v>
       </c>
       <c r="G7" s="11">
         <f t="shared" si="1"/>
-        <v>8.3999999999999986</v>
+        <v>8.23536</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1920,11 +1920,11 @@
       </c>
       <c r="F8" s="12">
         <f>SUM(F2:F7)</f>
-        <v>148.5</v>
+        <v>145.58940000000004</v>
       </c>
       <c r="G8" s="12">
         <f>SUM(G2:G7)</f>
-        <v>415.8</v>
+        <v>407.65032000000002</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1933,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="11">
-        <v>25</v>
+        <v>24.51</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>